<commit_message>
Complete Test lab test cases
</commit_message>
<xml_diff>
--- a/Resources/testdata/test.xlsx
+++ b/Resources/testdata/test.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="enviornment" sheetId="2" r:id="rId1"/>
-    <sheet name="devices" sheetId="1" r:id="rId2"/>
-    <sheet name="yl_command" sheetId="4" r:id="rId3"/>
-    <sheet name="yl_command_test" sheetId="5" r:id="rId4"/>
+    <sheet name="appserver" sheetId="6" r:id="rId2"/>
+    <sheet name="devices" sheetId="1" r:id="rId3"/>
+    <sheet name="yl_command" sheetId="4" r:id="rId4"/>
+    <sheet name="yl_command_test" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="118">
   <si>
     <t>YL EID</t>
   </si>
@@ -43,9 +44,6 @@
     <t>http://10.10.20.152:83</t>
   </si>
   <si>
-    <t>9902000000002600</t>
-  </si>
-  <si>
     <t>GasMeter1</t>
   </si>
   <si>
@@ -82,9 +80,6 @@
     <t>FMSURL</t>
   </si>
   <si>
-    <t>1ebeadac071eb7d3dc962d7603309181</t>
-  </si>
-  <si>
     <t>c775cf20a052fce804617cbea5266ab3</t>
   </si>
   <si>
@@ -278,6 +273,105 @@
   </si>
   <si>
     <t>SET_SUMMATION_REPORT_INTERVAL</t>
+  </si>
+  <si>
+    <t>AS_DEV_EUI</t>
+  </si>
+  <si>
+    <t>AS_APP_EUI</t>
+  </si>
+  <si>
+    <t>AS_APP_KEY</t>
+  </si>
+  <si>
+    <t>AS_NODE_NAME</t>
+  </si>
+  <si>
+    <t>TEST TEST</t>
+  </si>
+  <si>
+    <t>AS_URL</t>
+  </si>
+  <si>
+    <t>https://10.10.20.152:8080</t>
+  </si>
+  <si>
+    <t>99020000000026e2</t>
+  </si>
+  <si>
+    <t>98e1f231eb6b45b6fe9a0345d6160f67</t>
+  </si>
+  <si>
+    <t>APP_UPDATE</t>
+  </si>
+  <si>
+    <t>APL-LMT-YL01-1.0.15-STB</t>
+  </si>
+  <si>
+    <t>7ff9010202000028</t>
+  </si>
+  <si>
+    <t>7ff9010202000036</t>
+  </si>
+  <si>
+    <t>7ff9010202000086</t>
+  </si>
+  <si>
+    <t>7ff9010202000100</t>
+  </si>
+  <si>
+    <t>7ff9010202000106</t>
+  </si>
+  <si>
+    <t>7ff9010202000108</t>
+  </si>
+  <si>
+    <t>7ff9010202000116</t>
+  </si>
+  <si>
+    <t>7ff9010202000153</t>
+  </si>
+  <si>
+    <t>7ff9010202000166</t>
+  </si>
+  <si>
+    <t>000f161202000005</t>
+  </si>
+  <si>
+    <t>000f161202000006</t>
+  </si>
+  <si>
+    <t>000f161202000028</t>
+  </si>
+  <si>
+    <t>000f161202000036</t>
+  </si>
+  <si>
+    <t>000f161202000086</t>
+  </si>
+  <si>
+    <t>000f161202000100</t>
+  </si>
+  <si>
+    <t>000f161202000106</t>
+  </si>
+  <si>
+    <t>000f161202000108</t>
+  </si>
+  <si>
+    <t>000f161202000116</t>
+  </si>
+  <si>
+    <t>000f161202000153</t>
+  </si>
+  <si>
+    <t>000f161202000166</t>
+  </si>
+  <si>
+    <t>8000000000000001</t>
+  </si>
+  <si>
+    <t>2b7e151628aed2a6abf7158809cf4f3c</t>
   </si>
 </sst>
 </file>
@@ -358,7 +452,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -371,6 +465,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -677,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,24 +790,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,10 +815,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>92</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,32 +826,32 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,10 +859,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,10 +870,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,11 +881,20 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>93</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -798,24 +903,172 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
-  <ignoredErrors>
-    <ignoredError sqref="B3" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -828,7 +1081,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B2">
         <v>8001</v>
@@ -836,53 +1089,80 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B3">
         <v>8002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="B4">
         <v>8003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="B5">
         <v>8004</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="B6">
         <v>8005</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="B7">
         <v>8006</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>100</v>
+      </c>
       <c r="B8">
         <v>8007</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="B9">
         <v>8008</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>102</v>
+      </c>
       <c r="B10">
         <v>8009</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>103</v>
+      </c>
       <c r="B11">
         <v>8010</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="B12">
         <v>8011</v>
       </c>
@@ -892,12 +1172,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,443 +1188,443 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="6"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="6"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" s="6"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="6"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" s="6"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B29" s="6"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B31" s="6"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33" s="6"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" s="6"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B37" s="6"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B39" s="6"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="6"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B43" s="6"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B45" s="6"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="6"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B47" s="6"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B49" s="6"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B51" s="6"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B52" s="6"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B54" s="6"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B56" s="6"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B58" s="6"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B60" s="6"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B62" s="6"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B64" s="6"/>
     </row>
@@ -1353,7 +1633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1369,24 +1649,24 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="6"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
library updates with test server parameter removal
</commit_message>
<xml_diff>
--- a/Resources/testdata/test.xlsx
+++ b/Resources/testdata/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="enviornment" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="devices" sheetId="1" r:id="rId3"/>
     <sheet name="yl_command" sheetId="4" r:id="rId4"/>
     <sheet name="yl_command_test" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="122211" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="282">
   <si>
     <t>YL EID</t>
   </si>
@@ -263,12 +264,6 @@
     <t>pilot_light_mode=1,pilot_flow_min=13,pilot_flow_max=53</t>
   </si>
   <si>
-    <t>7ff9010202000005</t>
-  </si>
-  <si>
-    <t>7ff9010202000006</t>
-  </si>
-  <si>
     <t>GET_PRESSURE_ALARM_LEVEL_HIGH</t>
   </si>
   <si>
@@ -287,91 +282,589 @@
     <t>AS_NODE_NAME</t>
   </si>
   <si>
-    <t>TEST TEST</t>
-  </si>
-  <si>
     <t>AS_URL</t>
   </si>
   <si>
+    <t>99020000000026e2</t>
+  </si>
+  <si>
+    <t>98e1f231eb6b45b6fe9a0345d6160f67</t>
+  </si>
+  <si>
+    <t>APP_UPDATE</t>
+  </si>
+  <si>
+    <t>APL-LMT-YL01-1.0.15-STB</t>
+  </si>
+  <si>
+    <t>000f161202000028</t>
+  </si>
+  <si>
+    <t>000f161202000036</t>
+  </si>
+  <si>
+    <t>000f161202000086</t>
+  </si>
+  <si>
+    <t>000f161202000100</t>
+  </si>
+  <si>
+    <t>000f161202000106</t>
+  </si>
+  <si>
+    <t>000f161202000108</t>
+  </si>
+  <si>
+    <t>000f161202000116</t>
+  </si>
+  <si>
+    <t>000f161202000153</t>
+  </si>
+  <si>
+    <t>000f161202000166</t>
+  </si>
+  <si>
+    <t>8000000000000001</t>
+  </si>
+  <si>
+    <t>2b7e151628aed2a6abf7158809cf4f3c</t>
+  </si>
+  <si>
+    <t>000f161202000012</t>
+  </si>
+  <si>
+    <t>000f161202000013</t>
+  </si>
+  <si>
+    <t>000f161202000014</t>
+  </si>
+  <si>
+    <t>000f161202000016</t>
+  </si>
+  <si>
+    <t>000f161202000017</t>
+  </si>
+  <si>
+    <t>000f161202000021</t>
+  </si>
+  <si>
+    <t>000f161202000022</t>
+  </si>
+  <si>
+    <t>000f161202000024</t>
+  </si>
+  <si>
+    <t>000f161202000025</t>
+  </si>
+  <si>
+    <t>000f161202000026</t>
+  </si>
+  <si>
+    <t>000f161202000027</t>
+  </si>
+  <si>
+    <t>000f161202000030</t>
+  </si>
+  <si>
+    <t>000f161202000031</t>
+  </si>
+  <si>
+    <t>000f161202000032</t>
+  </si>
+  <si>
+    <t>000f161202000037</t>
+  </si>
+  <si>
+    <t>000f161202000081</t>
+  </si>
+  <si>
+    <t>000f161202000082</t>
+  </si>
+  <si>
+    <t>000f161202000083</t>
+  </si>
+  <si>
+    <t>000f161202000084</t>
+  </si>
+  <si>
+    <t>000f161202000085</t>
+  </si>
+  <si>
+    <t>000f161202000087</t>
+  </si>
+  <si>
+    <t>000f161202000088</t>
+  </si>
+  <si>
+    <t>000f161202000090</t>
+  </si>
+  <si>
+    <t>000f161202000092</t>
+  </si>
+  <si>
+    <t>000f161202000095</t>
+  </si>
+  <si>
+    <t>000f161202000097</t>
+  </si>
+  <si>
+    <t>000f161202000098</t>
+  </si>
+  <si>
+    <t>000f161202000102</t>
+  </si>
+  <si>
+    <t>000f161202000103</t>
+  </si>
+  <si>
+    <t>000f161202000104</t>
+  </si>
+  <si>
+    <t>000f161202000107</t>
+  </si>
+  <si>
+    <t>000f161202000112</t>
+  </si>
+  <si>
+    <t>000f161202000113</t>
+  </si>
+  <si>
+    <t>000f161202000117</t>
+  </si>
+  <si>
+    <t>000f161202000118</t>
+  </si>
+  <si>
+    <t>000f161202000161</t>
+  </si>
+  <si>
+    <t>000f161202000162</t>
+  </si>
+  <si>
+    <t>000f161202000163</t>
+  </si>
+  <si>
+    <t>000f161202000164</t>
+  </si>
+  <si>
+    <t>000f161202000165</t>
+  </si>
+  <si>
+    <t>7ff9011202000012</t>
+  </si>
+  <si>
+    <t>7ff9011202000013</t>
+  </si>
+  <si>
+    <t>7ff9011202000014</t>
+  </si>
+  <si>
+    <t>7ff9011202000016</t>
+  </si>
+  <si>
+    <t>7ff9011202000017</t>
+  </si>
+  <si>
+    <t>7ff9011202000021</t>
+  </si>
+  <si>
+    <t>7ff9011202000022</t>
+  </si>
+  <si>
+    <t>7ff9011202000024</t>
+  </si>
+  <si>
+    <t>7ff9011202000025</t>
+  </si>
+  <si>
+    <t>7ff9011202000026</t>
+  </si>
+  <si>
+    <t>7ff9011202000027</t>
+  </si>
+  <si>
+    <t>7ff9011202000028</t>
+  </si>
+  <si>
+    <t>7ff9011202000030</t>
+  </si>
+  <si>
+    <t>7ff9011202000031</t>
+  </si>
+  <si>
+    <t>7ff9011202000032</t>
+  </si>
+  <si>
+    <t>7ff9011202000036</t>
+  </si>
+  <si>
+    <t>7ff9011202000037</t>
+  </si>
+  <si>
+    <t>7ff9011202000081</t>
+  </si>
+  <si>
+    <t>7ff9011202000082</t>
+  </si>
+  <si>
+    <t>7ff9011202000083</t>
+  </si>
+  <si>
+    <t>7ff9011202000084</t>
+  </si>
+  <si>
+    <t>7ff9011202000085</t>
+  </si>
+  <si>
+    <t>7ff9011202000086</t>
+  </si>
+  <si>
+    <t>7ff9011202000087</t>
+  </si>
+  <si>
+    <t>7ff9011202000088</t>
+  </si>
+  <si>
+    <t>7ff9011202000090</t>
+  </si>
+  <si>
+    <t>7ff9011202000092</t>
+  </si>
+  <si>
+    <t>7ff9011202000095</t>
+  </si>
+  <si>
+    <t>7ff9011202000097</t>
+  </si>
+  <si>
+    <t>7ff9011202000098</t>
+  </si>
+  <si>
+    <t>7ff9011202000100</t>
+  </si>
+  <si>
+    <t>7ff9011202000102</t>
+  </si>
+  <si>
+    <t>7ff9011202000103</t>
+  </si>
+  <si>
+    <t>7ff9011202000104</t>
+  </si>
+  <si>
+    <t>7ff9011202000106</t>
+  </si>
+  <si>
+    <t>7ff9011202000107</t>
+  </si>
+  <si>
+    <t>7ff9011202000108</t>
+  </si>
+  <si>
+    <t>7ff9011202000112</t>
+  </si>
+  <si>
+    <t>7ff9011202000113</t>
+  </si>
+  <si>
+    <t>7ff9011202000116</t>
+  </si>
+  <si>
+    <t>7ff9011202000117</t>
+  </si>
+  <si>
+    <t>7ff9011202000118</t>
+  </si>
+  <si>
+    <t>7ff9011202000153</t>
+  </si>
+  <si>
+    <t>7ff9011202000161</t>
+  </si>
+  <si>
+    <t>7ff9011202000162</t>
+  </si>
+  <si>
+    <t>7ff9011202000163</t>
+  </si>
+  <si>
+    <t>7ff9011202000164</t>
+  </si>
+  <si>
+    <t>7ff9011202000165</t>
+  </si>
+  <si>
+    <t>7ff9011202000166</t>
+  </si>
+  <si>
+    <t>http://10.10.20.208:83</t>
+  </si>
+  <si>
+    <t>99020000000026e5</t>
+  </si>
+  <si>
+    <t>8858f181bf5e98779ed0723b02e232ab</t>
+  </si>
+  <si>
+    <t>000f161202000055</t>
+  </si>
+  <si>
+    <t>000f161202000064</t>
+  </si>
+  <si>
+    <t>000f161202000043</t>
+  </si>
+  <si>
+    <t>000f161202000061</t>
+  </si>
+  <si>
+    <t>000f161202000042</t>
+  </si>
+  <si>
+    <t>000f161202000059</t>
+  </si>
+  <si>
+    <t>000f161202000045</t>
+  </si>
+  <si>
+    <t>000f161202000069</t>
+  </si>
+  <si>
+    <t>000f161202000039</t>
+  </si>
+  <si>
+    <t>000f161202000074</t>
+  </si>
+  <si>
+    <t>000f161202000038</t>
+  </si>
+  <si>
+    <t>000f161202000040</t>
+  </si>
+  <si>
+    <t>000f161202000050</t>
+  </si>
+  <si>
+    <t>000f161202000073</t>
+  </si>
+  <si>
+    <t>000f161202000067</t>
+  </si>
+  <si>
+    <t>000f161202000049</t>
+  </si>
+  <si>
+    <t>000f161202000129</t>
+  </si>
+  <si>
+    <t>000f161202000060</t>
+  </si>
+  <si>
+    <t>000f161202000141</t>
+  </si>
+  <si>
+    <t>000f161202000151</t>
+  </si>
+  <si>
+    <t>000f161202000056</t>
+  </si>
+  <si>
+    <t>000f161202000121</t>
+  </si>
+  <si>
+    <t>000f161202000058</t>
+  </si>
+  <si>
+    <t>000f161202000123</t>
+  </si>
+  <si>
+    <t>000f161202000053</t>
+  </si>
+  <si>
+    <t>000f161202000147</t>
+  </si>
+  <si>
+    <t>000f161202000136</t>
+  </si>
+  <si>
+    <t>000f161202000134</t>
+  </si>
+  <si>
+    <t>000f161202000146</t>
+  </si>
+  <si>
+    <t>000f161202000132</t>
+  </si>
+  <si>
+    <t>000f161202000139</t>
+  </si>
+  <si>
+    <t>000f161202000156</t>
+  </si>
+  <si>
+    <t>000f161202000137</t>
+  </si>
+  <si>
+    <t>000f161202000131</t>
+  </si>
+  <si>
+    <t>000f161202000077</t>
+  </si>
+  <si>
+    <t>000f161202000057</t>
+  </si>
+  <si>
+    <t>000f161202000138</t>
+  </si>
+  <si>
+    <t>000f161202000126</t>
+  </si>
+  <si>
+    <t>7ff9011202000055</t>
+  </si>
+  <si>
+    <t>7ff9011202000064</t>
+  </si>
+  <si>
+    <t>7ff9011202000043</t>
+  </si>
+  <si>
+    <t>7ff9011202000061</t>
+  </si>
+  <si>
+    <t>7ff9011202000042</t>
+  </si>
+  <si>
+    <t>7ff9011202000059</t>
+  </si>
+  <si>
+    <t>7ff9011202000045</t>
+  </si>
+  <si>
+    <t>7ff9011202000069</t>
+  </si>
+  <si>
+    <t>7ff9011202000039</t>
+  </si>
+  <si>
+    <t>7ff9011202000074</t>
+  </si>
+  <si>
+    <t>7ff9011202000038</t>
+  </si>
+  <si>
+    <t>7ff9011202000040</t>
+  </si>
+  <si>
+    <t>7ff9011202000050</t>
+  </si>
+  <si>
+    <t>7ff9011202000073</t>
+  </si>
+  <si>
+    <t>7ff9011202000067</t>
+  </si>
+  <si>
+    <t>7ff9011202000049</t>
+  </si>
+  <si>
+    <t>7ff9011202000129</t>
+  </si>
+  <si>
+    <t>7ff9011202000060</t>
+  </si>
+  <si>
+    <t>7ff9011202000141</t>
+  </si>
+  <si>
+    <t>7ff9011202000151</t>
+  </si>
+  <si>
+    <t>7ff9011202000056</t>
+  </si>
+  <si>
+    <t>7ff9011202000121</t>
+  </si>
+  <si>
+    <t>7ff9011202000058</t>
+  </si>
+  <si>
+    <t>7ff9011202000123</t>
+  </si>
+  <si>
+    <t>7ff9011202000053</t>
+  </si>
+  <si>
+    <t>7ff9011202000147</t>
+  </si>
+  <si>
+    <t>7ff9011202000136</t>
+  </si>
+  <si>
+    <t>7ff9011202000134</t>
+  </si>
+  <si>
+    <t>7ff9011202000146</t>
+  </si>
+  <si>
+    <t>7ff9011202000132</t>
+  </si>
+  <si>
+    <t>7ff9011202000139</t>
+  </si>
+  <si>
+    <t>7ff9011202000156</t>
+  </si>
+  <si>
+    <t>7ff9011202000137</t>
+  </si>
+  <si>
+    <t>7ff9011202000131</t>
+  </si>
+  <si>
+    <t>7ff9011202000077</t>
+  </si>
+  <si>
+    <t>7ff9011202000057</t>
+  </si>
+  <si>
+    <t>7ff9011202000138</t>
+  </si>
+  <si>
+    <t>7ff9011202000126</t>
+  </si>
+  <si>
+    <t>DEV SERVER</t>
+  </si>
+  <si>
+    <t>MC DEV EUI</t>
+  </si>
+  <si>
+    <t>YL DEV EUI</t>
+  </si>
+  <si>
     <t>https://10.10.20.152:8080</t>
   </si>
   <si>
-    <t>99020000000026e2</t>
-  </si>
-  <si>
-    <t>98e1f231eb6b45b6fe9a0345d6160f67</t>
-  </si>
-  <si>
-    <t>APP_UPDATE</t>
-  </si>
-  <si>
-    <t>APL-LMT-YL01-1.0.15-STB</t>
-  </si>
-  <si>
-    <t>7ff9010202000028</t>
-  </si>
-  <si>
-    <t>7ff9010202000036</t>
-  </si>
-  <si>
-    <t>7ff9010202000086</t>
-  </si>
-  <si>
-    <t>7ff9010202000100</t>
-  </si>
-  <si>
-    <t>7ff9010202000106</t>
-  </si>
-  <si>
-    <t>7ff9010202000108</t>
-  </si>
-  <si>
-    <t>7ff9010202000116</t>
-  </si>
-  <si>
-    <t>7ff9010202000153</t>
-  </si>
-  <si>
-    <t>7ff9010202000166</t>
-  </si>
-  <si>
-    <t>000f161202000005</t>
-  </si>
-  <si>
-    <t>000f161202000006</t>
-  </si>
-  <si>
-    <t>000f161202000028</t>
-  </si>
-  <si>
-    <t>000f161202000036</t>
-  </si>
-  <si>
-    <t>000f161202000086</t>
-  </si>
-  <si>
-    <t>000f161202000100</t>
-  </si>
-  <si>
-    <t>000f161202000106</t>
-  </si>
-  <si>
-    <t>000f161202000108</t>
-  </si>
-  <si>
-    <t>000f161202000116</t>
-  </si>
-  <si>
-    <t>000f161202000153</t>
-  </si>
-  <si>
-    <t>000f161202000166</t>
-  </si>
-  <si>
-    <t>8000000000000001</t>
-  </si>
-  <si>
-    <t>2b7e151628aed2a6abf7158809cf4f3c</t>
+    <t>000f161202000167</t>
+  </si>
+  <si>
+    <t>7ff9011202000167</t>
+  </si>
+  <si>
+    <t>MC NIC</t>
+  </si>
+  <si>
+    <t>AS_SERVER_URL</t>
+  </si>
+  <si>
+    <t>https://10.10.20.125:8080</t>
+  </si>
+  <si>
+    <t>https://10.10.20.208:8080</t>
+  </si>
+  <si>
+    <t>000f161202999999</t>
   </si>
 </sst>
 </file>
@@ -410,7 +903,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +913,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -452,21 +951,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -773,10 +1273,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,11 +1284,11 @@
     <col min="1" max="1" width="21.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -798,8 +1298,11 @@
       <c r="C1" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>19</v>
       </c>
@@ -809,19 +1312,25 @@
       <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -831,8 +1340,11 @@
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -842,8 +1354,11 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -853,8 +1368,11 @@
       <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -864,8 +1382,11 @@
       <c r="C7" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -875,43 +1396,68 @@
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>280</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="B11" r:id="rId4"/>
+    <hyperlink ref="C11" r:id="rId5"/>
+    <hyperlink ref="D11" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,131 +1467,265 @@
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>105</v>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>281</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+        <v>277</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" s="5" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="5" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="5" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="5" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="5" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G14" s="5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="5" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="5" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="5" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="5" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="5" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="5" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="5" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="5" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="5" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="5" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="5" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="5" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="5" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="5" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="5" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="5" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="5"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1061,7 +1741,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1080,89 +1760,56 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="B2">
         <v>8001</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>82</v>
-      </c>
       <c r="B3">
         <v>8002</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="B4">
         <v>8003</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="B5">
         <v>8004</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="B6">
         <v>8005</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="B7">
         <v>8006</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="B8">
         <v>8007</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="B9">
         <v>8008</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="B10">
         <v>8009</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>103</v>
-      </c>
       <c r="B11">
         <v>8010</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="B12">
         <v>8011</v>
       </c>
@@ -1195,438 +1842,438 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="5"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="5"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="6"/>
+      <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="6"/>
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="6"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="6"/>
+      <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B25" s="6"/>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="6"/>
+      <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="5"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="6"/>
+      <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B35" s="6"/>
+      <c r="A35" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="6"/>
+      <c r="A37" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" s="5"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="5"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="6"/>
+      <c r="B41" s="5"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="6"/>
+      <c r="B43" s="5"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="6"/>
+      <c r="B45" s="5"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="6"/>
+      <c r="B46" s="5"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="6"/>
+      <c r="B47" s="5"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="6"/>
+      <c r="B49" s="5"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B51" s="6"/>
+      <c r="B51" s="5"/>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B52" s="6"/>
+      <c r="B52" s="5"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B54" s="6"/>
+      <c r="B54" s="5"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B55" s="6" t="s">
+      <c r="B55" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B56" s="6"/>
+      <c r="B56" s="5"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B58" s="6"/>
+      <c r="B58" s="5"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B60" s="6"/>
+      <c r="B60" s="5"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="6"/>
+      <c r="B62" s="5"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="A64" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="6"/>
+      <c r="B64" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1656,17 +2303,711 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="6"/>
+      <c r="A2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>